<commit_message>
domains: filtering by PID list in separate file
</commit_message>
<xml_diff>
--- a/R/count_domains_data/Protein interaction domain accession mod.xlsx
+++ b/R/count_domains_data/Protein interaction domain accession mod.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="453">
   <si>
     <t>IQ motif, EF-hand binding site</t>
   </si>
@@ -1783,7 +1783,7 @@
   <dimension ref="A1:D293"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1920,11 +1920,23 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1942,11 +1954,23 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>